<commit_message>
Updated on 01/05/21 (assignment still in progress)
</commit_message>
<xml_diff>
--- a/HTML/img/moviecovers/Dates in Movies.xlsx
+++ b/HTML/img/moviecovers/Dates in Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Documents\workshop_intec\HTML\img\moviecovers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A803C1FE-066E-439E-BEB5-B50D0295590E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9153FB4F-7814-495A-BE7C-464FFBB4B11C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{BD321F96-B228-4392-BB74-5A5D28048CD9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="206">
   <si>
     <t>Alien Invasion</t>
   </si>
@@ -519,9 +519,6 @@
     <t>Wife Type</t>
   </si>
   <si>
-    <t>Dec 10</t>
-  </si>
-  <si>
     <t>Abyss</t>
   </si>
   <si>
@@ -643,6 +640,12 @@
   </si>
   <si>
     <t>Seven Angry Men</t>
+  </si>
+  <si>
+    <t>December 10</t>
+  </si>
+  <si>
+    <t>Galactic Angel</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A8B062-760A-4715-9DBF-39A789787A78}">
   <dimension ref="A1:B135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1164,7 @@
         <v>162</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>163</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1222,10 +1225,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>185</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1270,10 +1273,10 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1342,18 +1345,18 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>181</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1382,7 +1385,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>125</v>
@@ -1390,7 +1393,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>125</v>
@@ -1398,7 +1401,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>125</v>
@@ -1414,18 +1417,18 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1542,10 +1545,10 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1574,10 +1577,10 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1606,7 +1609,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>13</v>
@@ -1614,10 +1617,10 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1654,7 +1657,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>47</v>
@@ -1726,7 +1729,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>7</v>
@@ -1742,15 +1745,15 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B84" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>81</v>
@@ -1782,10 +1785,10 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -1806,7 +1809,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>116</v>
@@ -1814,10 +1817,10 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B93" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -2070,7 +2073,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>3</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>3</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>3</v>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>3</v>
@@ -2102,7 +2105,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>3</v>
@@ -2110,7 +2113,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>3</v>
@@ -2118,7 +2121,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>3</v>
@@ -2126,7 +2129,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>3</v>
@@ -2134,7 +2137,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>3</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>3</v>
@@ -2150,7 +2153,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated on 03/05/21 (assignment finished at last!)
</commit_message>
<xml_diff>
--- a/HTML/img/moviecovers/Dates in Movies.xlsx
+++ b/HTML/img/moviecovers/Dates in Movies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Documents\workshop_intec\HTML\img\moviecovers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9153FB4F-7814-495A-BE7C-464FFBB4B11C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2229C516-4C70-4B55-A900-7129F39F31AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{BD321F96-B228-4392-BB74-5A5D28048CD9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="206">
   <si>
     <t>Alien Invasion</t>
   </si>
@@ -1067,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A8B062-760A-4715-9DBF-39A789787A78}">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1656,176 +1656,176 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>47</v>
+      <c r="A73" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" s="8" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>136</v>
+      <c r="A76" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>141</v>
+      <c r="A77" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>83</v>
+      <c r="A78" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="A79" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B80" s="4" t="s">
+      <c r="A80" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="5" t="s">
+      <c r="A81" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>7</v>
+      <c r="A82" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>25</v>
+      <c r="A83" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>173</v>
+      <c r="A84" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>81</v>
+      <c r="A85" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>160</v>
+      <c r="A86" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>66</v>
+      <c r="A87" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>78</v>
+      <c r="A88" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>192</v>
+      <c r="A89" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>92</v>
+      <c r="A90" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B91" s="6" t="s">
+      <c r="A91" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>177</v>
+      <c r="A93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>3</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>3</v>
@@ -1841,23 +1841,23 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B97" s="1" t="s">
+      <c r="A97" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>3</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>3</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>3</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>3</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>3</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>3</v>
@@ -1905,39 +1905,39 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B105" s="3" t="s">
+      <c r="A105" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B107" s="4" t="s">
+      <c r="A107" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="5" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>3</v>
@@ -1945,31 +1945,31 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B110" s="5" t="s">
+      <c r="A110" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B111" s="6" t="s">
+      <c r="A111" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>3</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="7" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>3</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>3</v>
@@ -1993,7 +1993,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>3</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>3</v>
@@ -2009,7 +2009,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="7" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>3</v>
@@ -2017,23 +2017,23 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B119" s="7" t="s">
+      <c r="A119" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B120" s="8" t="s">
         <v>3</v>
@@ -2041,7 +2041,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>3</v>
@@ -2049,7 +2049,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>3</v>
@@ -2057,39 +2057,39 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="8" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B124" s="8" t="s">
+      <c r="A124" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B126" s="9" t="s">
+      <c r="A126" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B126" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>3</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>3</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>3</v>
@@ -2113,7 +2113,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>3</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>3</v>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>3</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>3</v>
@@ -2145,23 +2145,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B135">
-    <sortCondition ref="B1:B135"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B134">
+    <sortCondition ref="B1:B134"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>